<commit_message>
almost done with analysis, left report writing
</commit_message>
<xml_diff>
--- a/Product_Survey_Results_Modified.xlsx
+++ b/Product_Survey_Results_Modified.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eugene\Desktop\Machine Intelligence\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiji\Documents\GitHub\MA4829_MachineIntelligence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C562275D-6632-47C2-80B0-CE06C39F3592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C591B342-786A-4833-87E2-91579861495C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer preference in a car" sheetId="1" r:id="rId1"/>
@@ -1323,39 +1323,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.625" customWidth="1"/>
-    <col min="9" max="9" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="19.625" customWidth="1"/>
-    <col min="14" max="14" width="67.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" customWidth="1"/>
+    <col min="9" max="9" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="19.59765625" customWidth="1"/>
+    <col min="14" max="14" width="67.69921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.59765625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.5" customWidth="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.625" customWidth="1"/>
-    <col min="24" max="24" width="72.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="66.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.59765625" customWidth="1"/>
+    <col min="24" max="24" width="72.3984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="66.3984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="52.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="102" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>89</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>93</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>95</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>96</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>97</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>98</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>100</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>101</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>102</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>103</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>104</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>107</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>108</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>109</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>111</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>113</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>114</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>115</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>116</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>117</v>
       </c>
@@ -7577,7 +7577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>118</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>119</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>120</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>120</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>121</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>122</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>123</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>124</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>125</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>126</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>127</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>128</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>129</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>130</v>
       </c>
@@ -8739,7 +8739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>131</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>132</v>
       </c>
@@ -8988,7 +8988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>134</v>
       </c>
@@ -9154,7 +9154,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>135</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>136</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>137</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>138</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>139</v>
       </c>
@@ -9569,7 +9569,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>140</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>141</v>
       </c>

</xml_diff>